<commit_message>
add in some check files
</commit_message>
<xml_diff>
--- a/pyeconlab/trade/dataset/NBERFeenstraWTF/meta/xlsx/intertemporal_eiso3n.xlsx
+++ b/pyeconlab/trade/dataset/NBERFeenstraWTF/meta/xlsx/intertemporal_eiso3n.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1231,8 +1231,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1296,6 +1296,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1374,6 +1379,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1408,6 +1414,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1583,14 +1590,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:XFD66"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="C1" s="1">
         <v>1962</v>
       </c>
@@ -1709,7 +1721,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1717,7 +1729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1842,7 +1854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1923,7 +1935,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1974,7 +1986,7 @@
       <c r="AN5" s="2"/>
       <c r="AO5" s="2"/>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2099,7 +2111,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2224,7 +2236,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2349,7 +2361,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2474,7 +2486,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -2599,7 +2611,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2664,7 +2676,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -2789,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -2866,7 +2878,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="14" spans="1:41">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -2991,7 +3003,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -3116,7 +3128,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -3181,7 +3193,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:41">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -3306,7 +3318,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:41">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -3431,7 +3443,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:41">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -3536,7 +3548,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:41">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -3661,7 +3673,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:41">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -3726,7 +3738,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:41">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -3851,7 +3863,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:41">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -3970,7 +3982,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:41">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -4095,7 +4107,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:41">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -4220,7 +4232,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:41">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -4345,7 +4357,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:41">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -4410,7 +4422,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:41">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -4477,7 +4489,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:41">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -4602,7 +4614,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:41">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -4727,7 +4739,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:41">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -4852,7 +4864,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="32" spans="1:41">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -4977,7 +4989,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:41">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -5030,7 +5042,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="34" spans="1:41">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -5155,7 +5167,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:41">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -5280,7 +5292,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:41">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -5405,7 +5417,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:41">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -5456,7 +5468,7 @@
       <c r="AN37" s="2"/>
       <c r="AO37" s="2"/>
     </row>
-    <row r="38" spans="1:41">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -5581,7 +5593,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:41">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -5706,7 +5718,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:41">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -5831,7 +5843,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:41">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -5956,7 +5968,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:41">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -6017,7 +6029,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="1:41">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -6142,7 +6154,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="44" spans="1:41">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -6265,7 +6277,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="45" spans="1:41">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -6316,7 +6328,7 @@
       <c r="AN45" s="2"/>
       <c r="AO45" s="2"/>
     </row>
-    <row r="46" spans="1:41">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -6441,7 +6453,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:41">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -6566,7 +6578,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="48" spans="1:41">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -6691,7 +6703,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="49" spans="1:41">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -6816,7 +6828,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="50" spans="1:41">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -6881,7 +6893,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="51" spans="1:41">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -7006,7 +7018,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="52" spans="1:41">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -7131,7 +7143,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="53" spans="1:41">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -7194,7 +7206,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="54" spans="1:41">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -7303,7 +7315,7 @@
       <c r="AN54" s="2"/>
       <c r="AO54" s="2"/>
     </row>
-    <row r="55" spans="1:41">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -7428,7 +7440,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="1:41">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -7553,7 +7565,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="57" spans="1:41">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -7678,7 +7690,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="58" spans="1:41">
+    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -7803,7 +7815,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:41">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -7852,7 +7864,7 @@
       <c r="AN59" s="2"/>
       <c r="AO59" s="2"/>
     </row>
-    <row r="60" spans="1:41">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -7907,7 +7919,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="61" spans="1:41">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -8032,7 +8044,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:41">
+    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -8157,7 +8169,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="63" spans="1:41">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -8282,7 +8294,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="64" spans="1:41">
+    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -8407,7 +8419,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="65" spans="1:41">
+    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -8472,7 +8484,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="66" spans="1:41">
+    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -8597,7 +8609,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="67" spans="1:41">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -8678,7 +8690,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="68" spans="1:41">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -8787,7 +8799,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="69" spans="1:41">
+    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -8912,7 +8924,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="70" spans="1:41">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -9037,7 +9049,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="71" spans="1:41">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -9142,7 +9154,7 @@
       <c r="AN71" s="2"/>
       <c r="AO71" s="2"/>
     </row>
-    <row r="72" spans="1:41">
+    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
@@ -9247,7 +9259,7 @@
       <c r="AN72" s="2"/>
       <c r="AO72" s="2"/>
     </row>
-    <row r="73" spans="1:41">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -9354,7 +9366,7 @@
       <c r="AN73" s="2"/>
       <c r="AO73" s="2"/>
     </row>
-    <row r="74" spans="1:41">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
@@ -9459,7 +9471,7 @@
       <c r="AN74" s="2"/>
       <c r="AO74" s="2"/>
     </row>
-    <row r="75" spans="1:41">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
@@ -9564,7 +9576,7 @@
       <c r="AN75" s="2"/>
       <c r="AO75" s="2"/>
     </row>
-    <row r="76" spans="1:41">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
@@ -9671,7 +9683,7 @@
       <c r="AN76" s="2"/>
       <c r="AO76" s="2"/>
     </row>
-    <row r="77" spans="1:41">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -9796,7 +9808,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="78" spans="1:41">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
@@ -9921,7 +9933,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:41">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -10046,7 +10058,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="80" spans="1:41">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -10171,7 +10183,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="81" spans="1:41">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
@@ -10296,7 +10308,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="82" spans="1:41">
+    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
@@ -10361,7 +10373,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="83" spans="1:41">
+    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
@@ -10432,7 +10444,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="84" spans="1:41">
+    <row r="84" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
@@ -10557,7 +10569,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="85" spans="1:41">
+    <row r="85" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
@@ -10678,7 +10690,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="86" spans="1:41">
+    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
@@ -10803,7 +10815,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="87" spans="1:41">
+    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
@@ -10916,7 +10928,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="88" spans="1:41">
+    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
@@ -11041,7 +11053,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="89" spans="1:41">
+    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
@@ -11166,7 +11178,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="90" spans="1:41">
+    <row r="90" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
@@ -11291,7 +11303,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="91" spans="1:41">
+    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
@@ -11416,7 +11428,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="92" spans="1:41">
+    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
@@ -11541,7 +11553,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="93" spans="1:41">
+    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -11666,7 +11678,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="94" spans="1:41">
+    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
@@ -11791,7 +11803,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="95" spans="1:41">
+    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
@@ -11916,7 +11928,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="96" spans="1:41">
+    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
@@ -12041,7 +12053,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="97" spans="1:41">
+    <row r="97" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
@@ -12166,7 +12178,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="98" spans="1:41">
+    <row r="98" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
@@ -12291,7 +12303,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="99" spans="1:41">
+    <row r="99" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
@@ -12416,7 +12428,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="100" spans="1:41">
+    <row r="100" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
@@ -12541,7 +12553,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="101" spans="1:41">
+    <row r="101" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
@@ -12666,7 +12678,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="102" spans="1:41">
+    <row r="102" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>101</v>
       </c>
@@ -12791,7 +12803,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="103" spans="1:41">
+    <row r="103" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
@@ -12916,7 +12928,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="104" spans="1:41">
+    <row r="104" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>103</v>
       </c>
@@ -13041,7 +13053,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="105" spans="1:41">
+    <row r="105" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>104</v>
       </c>
@@ -13166,7 +13178,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="106" spans="1:41">
+    <row r="106" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>105</v>
       </c>
@@ -13291,7 +13303,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="107" spans="1:41">
+    <row r="107" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
@@ -13356,7 +13368,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="108" spans="1:41">
+    <row r="108" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
@@ -13481,7 +13493,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="109" spans="1:41">
+    <row r="109" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>108</v>
       </c>
@@ -13606,7 +13618,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="110" spans="1:41">
+    <row r="110" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>109</v>
       </c>
@@ -13731,7 +13743,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="111" spans="1:41">
+    <row r="111" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>110</v>
       </c>
@@ -13856,7 +13868,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="112" spans="1:41">
+    <row r="112" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
@@ -13981,7 +13993,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="113" spans="1:41">
+    <row r="113" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
@@ -14046,7 +14058,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="114" spans="1:41">
+    <row r="114" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
@@ -14097,7 +14109,7 @@
       </c>
       <c r="AO114" s="2"/>
     </row>
-    <row r="115" spans="1:41">
+    <row r="115" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>114</v>
       </c>
@@ -14222,7 +14234,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="116" spans="1:41">
+    <row r="116" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
@@ -14287,7 +14299,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="117" spans="1:41">
+    <row r="117" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>116</v>
       </c>
@@ -14412,7 +14424,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="118" spans="1:41">
+    <row r="118" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>117</v>
       </c>
@@ -14537,7 +14549,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="119" spans="1:41">
+    <row r="119" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>118</v>
       </c>
@@ -14662,7 +14674,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="120" spans="1:41">
+    <row r="120" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>119</v>
       </c>
@@ -14727,7 +14739,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="121" spans="1:41">
+    <row r="121" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
@@ -14852,7 +14864,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="122" spans="1:41">
+    <row r="122" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>121</v>
       </c>
@@ -14975,7 +14987,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="123" spans="1:41">
+    <row r="123" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>122</v>
       </c>
@@ -15100,7 +15112,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="124" spans="1:41">
+    <row r="124" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>123</v>
       </c>
@@ -15225,7 +15237,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="125" spans="1:41">
+    <row r="125" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
@@ -15350,7 +15362,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="126" spans="1:41">
+    <row r="126" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>125</v>
       </c>
@@ -15475,7 +15487,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="127" spans="1:41">
+    <row r="127" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>126</v>
       </c>
@@ -15600,7 +15612,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="128" spans="1:41">
+    <row r="128" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>127</v>
       </c>
@@ -15725,7 +15737,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="129" spans="1:41">
+    <row r="129" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>128</v>
       </c>
@@ -15850,7 +15862,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="130" spans="1:41">
+    <row r="130" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>129</v>
       </c>
@@ -15975,7 +15987,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="131" spans="1:41">
+    <row r="131" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>130</v>
       </c>
@@ -16100,7 +16112,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="132" spans="1:41">
+    <row r="132" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>131</v>
       </c>
@@ -16225,7 +16237,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="133" spans="1:41">
+    <row r="133" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>132</v>
       </c>
@@ -16350,7 +16362,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="134" spans="1:41">
+    <row r="134" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>133</v>
       </c>
@@ -16475,7 +16487,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="135" spans="1:41">
+    <row r="135" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>134</v>
       </c>
@@ -16600,7 +16612,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="136" spans="1:41">
+    <row r="136" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>135</v>
       </c>
@@ -16705,7 +16717,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="137" spans="1:41">
+    <row r="137" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>136</v>
       </c>
@@ -16830,7 +16842,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="138" spans="1:41">
+    <row r="138" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>137</v>
       </c>
@@ -16955,7 +16967,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="139" spans="1:41">
+    <row r="139" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>138</v>
       </c>
@@ -17080,7 +17092,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="140" spans="1:41">
+    <row r="140" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>139</v>
       </c>
@@ -17205,7 +17217,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="141" spans="1:41">
+    <row r="141" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>140</v>
       </c>
@@ -17330,7 +17342,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="142" spans="1:41">
+    <row r="142" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>141</v>
       </c>
@@ -17455,7 +17467,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="143" spans="1:41">
+    <row r="143" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>142</v>
       </c>
@@ -17504,7 +17516,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="144" spans="1:41">
+    <row r="144" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>143</v>
       </c>
@@ -17629,7 +17641,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="145" spans="1:41">
+    <row r="145" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>144</v>
       </c>
@@ -17710,7 +17722,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="146" spans="1:41">
+    <row r="146" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>145</v>
       </c>
@@ -17835,7 +17847,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="147" spans="1:41">
+    <row r="147" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>146</v>
       </c>
@@ -17960,7 +17972,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="148" spans="1:41">
+    <row r="148" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>147</v>
       </c>
@@ -18085,7 +18097,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="149" spans="1:41">
+    <row r="149" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>148</v>
       </c>
@@ -18210,7 +18222,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="150" spans="1:41">
+    <row r="150" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>149</v>
       </c>
@@ -18335,7 +18347,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="151" spans="1:41">
+    <row r="151" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>150</v>
       </c>
@@ -18460,7 +18472,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="152" spans="1:41">
+    <row r="152" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>151</v>
       </c>
@@ -18585,7 +18597,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="153" spans="1:41">
+    <row r="153" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>152</v>
       </c>
@@ -18710,7 +18722,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="154" spans="1:41">
+    <row r="154" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>153</v>
       </c>
@@ -18835,7 +18847,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="155" spans="1:41">
+    <row r="155" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>154</v>
       </c>
@@ -18900,7 +18912,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="156" spans="1:41">
+    <row r="156" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>155</v>
       </c>
@@ -19025,7 +19037,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="157" spans="1:41">
+    <row r="157" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>156</v>
       </c>
@@ -19096,7 +19108,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="158" spans="1:41">
+    <row r="158" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>157</v>
       </c>
@@ -19219,7 +19231,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="159" spans="1:41">
+    <row r="159" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>158</v>
       </c>
@@ -19344,7 +19356,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="160" spans="1:41">
+    <row r="160" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>159</v>
       </c>
@@ -19469,7 +19481,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="161" spans="1:41">
+    <row r="161" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>160</v>
       </c>
@@ -19594,7 +19606,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="162" spans="1:41">
+    <row r="162" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>161</v>
       </c>
@@ -19705,7 +19717,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="163" spans="1:41">
+    <row r="163" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>162</v>
       </c>
@@ -19830,7 +19842,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="164" spans="1:41">
+    <row r="164" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>163</v>
       </c>
@@ -19955,7 +19967,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="165" spans="1:41">
+    <row r="165" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>164</v>
       </c>
@@ -20022,7 +20034,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="166" spans="1:41">
+    <row r="166" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>165</v>
       </c>
@@ -20087,7 +20099,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="167" spans="1:41">
+    <row r="167" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>166</v>
       </c>
@@ -20212,7 +20224,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="168" spans="1:41">
+    <row r="168" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>167</v>
       </c>
@@ -20337,7 +20349,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="169" spans="1:41">
+    <row r="169" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>168</v>
       </c>
@@ -20462,7 +20474,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="170" spans="1:41">
+    <row r="170" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>169</v>
       </c>
@@ -20587,7 +20599,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="171" spans="1:41">
+    <row r="171" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>170</v>
       </c>
@@ -20696,7 +20708,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="172" spans="1:41">
+    <row r="172" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>171</v>
       </c>
@@ -20817,7 +20829,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="173" spans="1:41">
+    <row r="173" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>172</v>
       </c>
@@ -20942,7 +20954,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="174" spans="1:41">
+    <row r="174" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>173</v>
       </c>
@@ -21067,7 +21079,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="175" spans="1:41">
+    <row r="175" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>174</v>
       </c>
@@ -21192,7 +21204,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="176" spans="1:41">
+    <row r="176" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>175</v>
       </c>
@@ -21317,7 +21329,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="177" spans="1:41">
+    <row r="177" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>176</v>
       </c>
@@ -21442,7 +21454,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="178" spans="1:41">
+    <row r="178" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>177</v>
       </c>
@@ -21567,7 +21579,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="179" spans="1:41">
+    <row r="179" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>178</v>
       </c>
@@ -21630,7 +21642,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="180" spans="1:41">
+    <row r="180" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>179</v>
       </c>
@@ -21755,7 +21767,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="181" spans="1:41">
+    <row r="181" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>180</v>
       </c>
@@ -21820,7 +21832,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="182" spans="1:41">
+    <row r="182" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>181</v>
       </c>
@@ -21945,7 +21957,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="183" spans="1:41">
+    <row r="183" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>182</v>
       </c>
@@ -22070,7 +22082,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="184" spans="1:41">
+    <row r="184" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>183</v>
       </c>
@@ -22195,7 +22207,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="185" spans="1:41">
+    <row r="185" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>184</v>
       </c>
@@ -22320,7 +22332,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="186" spans="1:41">
+    <row r="186" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>185</v>
       </c>
@@ -22445,7 +22457,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="187" spans="1:41">
+    <row r="187" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>186</v>
       </c>
@@ -22570,7 +22582,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="188" spans="1:41">
+    <row r="188" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>187</v>
       </c>
@@ -22635,7 +22647,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="189" spans="1:41">
+    <row r="189" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>188</v>
       </c>
@@ -22760,7 +22772,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="190" spans="1:41">
+    <row r="190" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>189</v>
       </c>
@@ -22885,7 +22897,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="191" spans="1:41">
+    <row r="191" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>190</v>
       </c>
@@ -23010,7 +23022,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="192" spans="1:41">
+    <row r="192" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>191</v>
       </c>
@@ -23135,7 +23147,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="193" spans="1:41">
+    <row r="193" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>192</v>
       </c>
@@ -23206,7 +23218,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="194" spans="1:41">
+    <row r="194" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>193</v>
       </c>
@@ -23323,7 +23335,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="195" spans="1:41">
+    <row r="195" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>194</v>
       </c>
@@ -23448,7 +23460,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="196" spans="1:41">
+    <row r="196" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>195</v>
       </c>
@@ -23513,7 +23525,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="197" spans="1:41">
+    <row r="197" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>196</v>
       </c>
@@ -23638,7 +23650,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="198" spans="1:41">
+    <row r="198" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>197</v>
       </c>
@@ -23763,7 +23775,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="199" spans="1:41">
+    <row r="199" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>198</v>
       </c>
@@ -23888,7 +23900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:41">
+    <row r="200" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>199</v>
       </c>
@@ -23955,7 +23967,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="201" spans="1:41">
+    <row r="201" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>200</v>
       </c>
@@ -24026,7 +24038,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="202" spans="1:41">
+    <row r="202" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>201</v>
       </c>
@@ -24151,7 +24163,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="203" spans="1:41">
+    <row r="203" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>202</v>
       </c>

</xml_diff>